<commit_message>
UPDATE aggiornamento file excel
</commit_message>
<xml_diff>
--- a/Utils/Componenti da acquistare.xlsx
+++ b/Utils/Componenti da acquistare.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t xml:space="preserve">Componenti da acquistare</t>
   </si>
@@ -49,7 +49,8 @@
     <t xml:space="preserve">Consumi</t>
   </si>
   <si>
-    <t xml:space="preserve">ECHO Multibeam Imaging Sonar</t>
+    <t xml:space="preserve">ECHO Multibeam Imaging Sonar
+(Boost?)</t>
   </si>
   <si>
     <t xml:space="preserve">Sonoptix</t>
@@ -132,28 +133,24 @@
     <t xml:space="preserve">Stereo Camera (da scegliere 2 o 4mm)</t>
   </si>
   <si>
-    <t xml:space="preserve">1) ZED 2i (IP66)
-2) ZED X (IP67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) https://store.stereolabs.com/products/zed-2i?variant=41379929096348
-2) https://store.stereolabs.com/en-it/products/zed-x-stereo-camera?pr_prod_strat=pinned&amp;pr_rec_id=d28440251&amp;pr_rec_pid=7732260602012&amp;pr_ref_pid=4373392359555&amp;pr_seq=uniform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) $499,00 = €458.78
-2) €559,00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) 175.25 x 30.25 x 43.10 mm
-2)164 x 32 x 37 mm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) 166 g
-2) 240 g </t>
+    <t xml:space="preserve">ZED 2i (IP66)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://store.stereolabs.com/products/zed-2i?variant=41379929096348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€499,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">175.25 x 30.25 x 43.10 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166 g</t>
   </si>
   <si>
     <t xml:space="preserve">1) 5 V (via USB)
-2) 5 V (?)(via GMSL2)</t>
+</t>
   </si>
   <si>
     <t xml:space="preserve">2 W</t>
@@ -174,19 +171,65 @@
     <t xml:space="preserve">https://mimotore.com/products/dc-dc-converter-20a-300w-step-down-buck-boost-power-adjustable-charger-board?currency=EUR&amp;variant=45774090993986&amp;utm_medium=cpc&amp;utm_source=google&amp;utm_campaign=Google%20Shopping&amp;stkn=03c97ffecb69</t>
   </si>
   <si>
-    <t xml:space="preserve">tot. € 9.141,58 - 9241,80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tot. 1109-1183 g</t>
+    <t xml:space="preserve">Cilindro StereoCamera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bluerobotics.com/store/watertight-enclosures/locking-series/wte-locking-tube-r1-vp/
+Acrilico, 75 mm (diametro), 300mm (lunghezza)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$215.00=€197,71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">560 g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tappi Cilindro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bluerobotics.com/store/watertight-enclosures/locking-series/wte-end-cap-vp/ 
+Alluminio, 1x 4 fori, 1x senza fori, 75mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$28.00=€25,75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97 g + 102 g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS (da comprare?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ublox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://futuranet.it/prodotto/ublox-neo-6m-per-controller-di-volo-apm/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cilindro superiore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30x23x4 mm (modulo)
+25x25x8 mm (antenna)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-5 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tot. € 9426,26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tot. 1868 g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[RED]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$€-410]\ #,##0.00;[RED]\-[$€-410]\ #,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -271,7 +314,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,16 +335,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -382,17 +437,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="81.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.55"/>
@@ -431,20 +486,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -467,13 +522,13 @@
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -493,7 +548,7 @@
       <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -515,29 +570,29 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -548,7 +603,7 @@
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="7" t="n">
@@ -562,16 +617,73 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -580,6 +692,9 @@
     <hyperlink ref="C3" r:id="rId2" display="https://bluerobotics.com/store/comm-control-power/tether-interface/ethswitch/"/>
     <hyperlink ref="C4" r:id="rId3" display="https://mikrotik.com/product/RBGrooveA-52HPnr2"/>
     <hyperlink ref="C7" r:id="rId4" display="https://mimotore.com/products/dc-dc-converter-20a-300w-step-down-buck-boost-power-adjustable-charger-board?currency=EUR&amp;variant=45774090993986&amp;utm_medium=cpc&amp;utm_source=google&amp;utm_campaign=Google%20Shopping&amp;stkn=03c97ffecb69"/>
+    <hyperlink ref="C8" r:id="rId5" display="https://bluerobotics.com/store/watertight-enclosures/locking-series/wte-locking-tube-r1-vp/"/>
+    <hyperlink ref="C9" r:id="rId6" display="https://bluerobotics.com/store/watertight-enclosures/locking-series/wte-end-cap-vp/"/>
+    <hyperlink ref="C10" r:id="rId7" display="https://futuranet.it/prodotto/ublox-neo-6m-per-controller-di-volo-apm/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>